<commit_message>
Update Source Code and SRS Document
</commit_message>
<xml_diff>
--- a/SRS/Gantt Chart.xlsx
+++ b/SRS/Gantt Chart.xlsx
@@ -298,35 +298,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -623,138 +623,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="42.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9">
+      <c r="A19" s="6">
         <v>5</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <v>6</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="12" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update source code and Gantt Chart
</commit_message>
<xml_diff>
--- a/SRS/Gantt Chart.xlsx
+++ b/SRS/Gantt Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Công việc</t>
   </si>
@@ -122,63 +122,15 @@
     <t>Hệ thống hiển thị danh sách phòng trong cơ sở dữ liệu lên trang web</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Candara"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">Hệ thống thực hiện chức năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Candara"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>đăng ký, đăng nhập vào website đặt phòng và trang admin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hệ thống hiện danh sách phòng theo kết quả </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Candara"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>tìm kiếm</t>
-    </r>
-  </si>
-  <si>
     <t>Hệ thống cho phép đặt phòng</t>
   </si>
   <si>
     <t>Hệ thống hoàn thành test các chức năng trong website đặt phòng</t>
   </si>
   <si>
-    <t>Hệ thống cho phép admin quản lý đặt phòng</t>
-  </si>
-  <si>
-    <t>Tuần 8,9,10</t>
-  </si>
-  <si>
     <t>Thiết kế chi tiết giao diện chức năng đặt phòng</t>
   </si>
   <si>
-    <t>Tuần 5,6.7</t>
-  </si>
-  <si>
     <t>Phân tích chi tiết  (đặc tả use case)</t>
   </si>
   <si>
@@ -189,6 +141,33 @@
   </si>
   <si>
     <t xml:space="preserve">Trang giao diện HTML </t>
+  </si>
+  <si>
+    <t>Xử lý chức năng đăng ký thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Xử lý chức năng đăng nhập, đăng xuất thông tin người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xử lý chức năng hiển thị thông tin người dùng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống thực hiện chức năng đăng ký, đăng nhập vào website đặt phòng </t>
+  </si>
+  <si>
+    <t>Tuần 5,6</t>
+  </si>
+  <si>
+    <t>Tuần 7,8</t>
+  </si>
+  <si>
+    <t>Tuần 11,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xử lý chức năng hiển thị danh sách phòng </t>
+  </si>
+  <si>
+    <t>Xử lý chức năng hiển thị danh sách phòng theo từng loại phòng</t>
   </si>
 </sst>
 </file>
@@ -569,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -584,12 +563,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,15 +612,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,6 +686,27 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1008,19 +1005,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1034,317 +1031,321 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="39">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="13" t="s">
-        <v>40</v>
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="46"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="14" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="14" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="14" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="46"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="14" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="46"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="41"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="18" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="47"/>
+      <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>2</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="45" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="44" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="14" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="46"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="14" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="46"/>
+      <c r="E15" s="45"/>
     </row>
     <row r="16" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="41"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="47"/>
+      <c r="E16" s="46"/>
     </row>
     <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36">
+      <c r="A17" s="35">
         <v>3</v>
       </c>
-      <c r="B17" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="48" t="s">
-        <v>39</v>
+      <c r="E17" s="47" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="21" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="30"/>
     </row>
     <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="13" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27">
+      <c r="A20" s="24">
         <v>4</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>5</v>
+      </c>
+      <c r="B21" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="C21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="31"/>
-    </row>
-    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
-        <v>5</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="31"/>
-    </row>
-    <row r="22" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7">
+      <c r="E21" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="30"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="30"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="48">
         <v>6</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B24" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="C24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="31"/>
-    </row>
-    <row r="23" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
-        <v>7</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="32"/>
-    </row>
-    <row r="24" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
-        <v>8</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
-        <v>9</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>21</v>
+      <c r="E24" s="30"/>
+    </row>
+    <row r="25" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="31"/>
-    </row>
-    <row r="26" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12">
-        <v>10</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="15" t="s">
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10">
+        <v>8</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="32"/>
+        <v>14</v>
+      </c>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="16">
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E24:E26"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A16"/>
@@ -1353,7 +1354,9 @@
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="E3:E10"/>
     <mergeCell ref="E11:E16"/>
-    <mergeCell ref="E17:E23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E21:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Document and Gantt Chart
</commit_message>
<xml_diff>
--- a/SRS/Gantt Chart.xlsx
+++ b/SRS/Gantt Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Công việc</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Chức năng  Quản lý phòng, quản lý khách sạn</t>
   </si>
   <si>
-    <t xml:space="preserve">Test các chức năng </t>
-  </si>
-  <si>
     <t>Mục tiêu</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t xml:space="preserve">Xây dựng cơ sở dữ liệu </t>
   </si>
   <si>
-    <t xml:space="preserve">Giao diện và xử lý </t>
-  </si>
-  <si>
     <t>Hệ thống hiển thị danh sách phòng trong cơ sở dữ liệu lên trang web</t>
   </si>
   <si>
@@ -174,6 +168,27 @@
   </si>
   <si>
     <t>Tuần 9,10</t>
+  </si>
+  <si>
+    <t>Xử lý chọn phòng để vào Your Room của user</t>
+  </si>
+  <si>
+    <t>Xử lý thay đổi thông tin đặt phòng (số lượng, ngày check-in, check-out)</t>
+  </si>
+  <si>
+    <t>Xử lý thanh toán phòng đặt</t>
+  </si>
+  <si>
+    <t>Giao diện và xử lý thêm, xóa, sửa thông tin đặt phòng</t>
+  </si>
+  <si>
+    <t>Unit Test chức năng đặt phòng</t>
+  </si>
+  <si>
+    <t>Spring Test chức năng đặt phòng</t>
+  </si>
+  <si>
+    <t>Tuần 13,14</t>
   </si>
 </sst>
 </file>
@@ -554,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -569,20 +584,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -627,8 +633,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -637,6 +643,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,26 +717,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1008,20 +1020,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1034,338 +1046,371 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41">
+      <c r="A3" s="45">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="11" t="s">
-        <v>35</v>
+      <c r="A4" s="46"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="48"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="12" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="46"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="42"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="11" t="s">
-        <v>25</v>
+      <c r="A9" s="46"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="43"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="45">
+        <v>2</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="49"/>
-    </row>
-    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="41">
-        <v>2</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="47" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="42"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="12" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="12" t="s">
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="48"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="12" t="s">
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="48"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="12" t="s">
+      <c r="A15" s="46"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="48"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="15" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="49"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38">
+      <c r="A17" s="42">
         <v>3</v>
       </c>
-      <c r="B17" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="53" t="s">
-        <v>43</v>
+      <c r="E17" s="33" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="39"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="28"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="40"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="11" t="s">
-        <v>28</v>
+      <c r="A19" s="44"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23">
+      <c r="A20" s="20">
         <v>4</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="24">
+        <v>5</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="25"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="27">
-        <v>5</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+    </row>
+    <row r="23" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="36">
+        <v>6</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-    </row>
-    <row r="23" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-    </row>
-    <row r="24" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32">
-        <v>6</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="27" t="s">
-        <v>49</v>
+      <c r="E24" s="36" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="8" t="s">
-        <v>47</v>
+      <c r="A25" s="36"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="28"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10">
+      <c r="A26" s="24">
         <v>8</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="34" t="s">
         <v>30</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="28"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25"/>
-      <c r="B27" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>30</v>
+      <c r="B27" s="51"/>
+      <c r="C27" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="28"/>
-    </row>
-    <row r="28" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>9</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="E27" s="36"/>
+    </row>
+    <row r="28" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>45</v>
+      <c r="E28" s="36"/>
+    </row>
+    <row r="29" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="22">
+        <v>9</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="36"/>
+    </row>
+    <row r="30" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="24">
+        <v>10</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="26"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="D21:D23"/>
+  <mergeCells count="21">
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A24:A25"/>
@@ -1376,6 +1421,14 @@
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B16"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E24:E29"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>